<commit_message>
update version tracker to latest
</commit_message>
<xml_diff>
--- a/docs/Beam Version Tracker.xlsx
+++ b/docs/Beam Version Tracker.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27904"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://chapinhall.sharepoint.com/sites/ETL/Shared Documents/Record linkage/Project Management/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="554" documentId="11_45811371172ACF8F4E6E08FDBCD9810CE6C478D1" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C4FCB4D4-B397-4483-B680-6A6753A1BDAC}"/>
+  <xr:revisionPtr revIDLastSave="589" documentId="11_45811371172ACF8F4E6E08FDBCD9810CE6C478D1" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DA6E79E9-3742-49D5-8D1A-9B5706273361}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -57,27 +57,27 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="64">
   <si>
     <t>Last Update: 10/5/2023</t>
   </si>
   <si>
-    <t>v0</t>
-  </si>
-  <si>
-    <t>v1</t>
-  </si>
-  <si>
-    <t>v1.1</t>
-  </si>
-  <si>
-    <t>v1.2</t>
-  </si>
-  <si>
-    <t>v1.3 - IN REVIEW</t>
-  </si>
-  <si>
-    <t>v1.4 - FY24 CLEAN VERSION</t>
+    <t>v0 (archived)</t>
+  </si>
+  <si>
+    <t>v1 (archived)</t>
+  </si>
+  <si>
+    <t>v1.1 (archived)</t>
+  </si>
+  <si>
+    <t>v1.2 (archived)</t>
+  </si>
+  <si>
+    <t>v1.3 (archived)</t>
+  </si>
+  <si>
+    <t>v1.4 - CURRENT</t>
   </si>
   <si>
     <t>Short term goals 1</t>
@@ -165,14 +165,16 @@
 Functions for printing out record pairs for easy clerical review;</t>
   </si>
   <si>
-    <t>Clean up pipeline 
-Update workflow to have a csv path and a postgres path</t>
-  </si>
-  <si>
-    <t>AL - Round out workflow from raw data to end-product (including data storage, match vs project directory, server use, etc); [v1.4]
-AL - Clean up pipeline with new preprocessing component; [v1.4]
-SS - Handle matches with multiple IDs, potentially with different strengths (i.e. CHA undup); [in progress as part of the collaborative project]
-Working session - Draft and pilot match analysis to include in linkage memo;</t>
+    <t>Streamlined dedup blocking code
+Fixed bugs from upgrade to pandas 2
+Fixed bugs in 1:M match rate calculation</t>
+  </si>
+  <si>
+    <t>Update workflow to have a csv path and a postgres path
+Clean up pipeline to have better integration with the preprocessing component
+More user-friendly config (yaml files, split preprocessing, etc.)
+Handle matches with multiple IDs, potentially with different strengths
+Draft and pilot match analysis to include in linkage memo;</t>
   </si>
   <si>
     <t xml:space="preserve">Pilot sampling and reviewing functions to test what is desirable and how it could fit into the workflow;
@@ -194,9 +196,8 @@
     <t>Created full README</t>
   </si>
   <si>
-    <t>W/ Emily - Draft user manual;
-W/ Emily - Create tool name;
-W/ Emily - Collaborate on when/how sensitivity testing can happen (*Family Networks application)</t>
+    <t>Draft user manual;
+Planning for case studies of sensitivity testing</t>
   </si>
   <si>
     <t>Create working version of user manual</t>
@@ -275,22 +276,10 @@
     <t>n/a</t>
   </si>
   <si>
-    <t>https://chapinhall.sharepoint.com/:w:/r/sites/ETL/Shared%20Documents/Record%20linkage/Design/Record%20Linkage%20Tool%20Design%20(v1).docx?d=w21eeeadf8c274e96abd6dd02e716cc62&amp;csf=1&amp;web=1&amp;e=ZUVgZy</t>
-  </si>
-  <si>
-    <t>https://chapinhall.sharepoint.com/:w:/r/sites/ETL/Shared%20Documents/Record%20linkage/Design/Record%20Linkage%20v1.1%20Match%20Logic.docx?d=w547305039b2041518f0ccf48b2af8a42&amp;csf=1&amp;web=1&amp;e=msDBET</t>
-  </si>
-  <si>
     <t>Same as v1.1</t>
   </si>
   <si>
     <t>Link to commit</t>
-  </si>
-  <si>
-    <t>https://chudev01.chapinhall.org/record-linkage/record-linkage-v0/-/commit/0a7afb01842583e6b763db8fdd8ae0a9f9075b4d</t>
-  </si>
-  <si>
-    <t>https://chudev01.chapinhall.org/record-linkage/record-linkage-v0/-/commit/a2f4551b52914b4b2acf9159f2ee17a7cca53d88</t>
   </si>
   <si>
     <t>tbd</t>
@@ -855,8 +844,8 @@
   <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="D4" sqref="D4"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="D5" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="F5" sqref="F5"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
     </sheetView>
@@ -1088,41 +1077,35 @@
       <c r="B9" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="C9" s="7"/>
+      <c r="D9" s="14"/>
+      <c r="E9" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="D9" s="14" t="s">
-        <v>57</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>58</v>
-      </c>
       <c r="F9" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="G9" s="5"/>
+        <v>56</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>56</v>
+      </c>
       <c r="H9" s="18"/>
       <c r="I9" s="18"/>
       <c r="J9" s="18"/>
     </row>
     <row r="10" spans="1:10">
       <c r="A10" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="B10" s="14" t="s">
-        <v>60</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>61</v>
-      </c>
+        <v>57</v>
+      </c>
+      <c r="B10" s="14"/>
+      <c r="C10" s="6"/>
       <c r="D10" s="13" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="F10" s="13" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="G10" s="5"/>
       <c r="H10" s="18"/>
@@ -1131,19 +1114,19 @@
     </row>
     <row r="11" spans="1:10" ht="167.25">
       <c r="A11" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="B11" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="D11" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="E11" s="3" t="s">
         <v>63</v>
-      </c>
-      <c r="B11" s="12" t="s">
-        <v>64</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="D11" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>67</v>
       </c>
       <c r="F11" s="12"/>
       <c r="G11" s="3"/>
@@ -1153,15 +1136,9 @@
     </row>
   </sheetData>
   <autoFilter ref="A1" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
-  <hyperlinks>
-    <hyperlink ref="C10" r:id="rId1" xr:uid="{35D1EA8A-A0E9-46F7-9DA4-328960C2EE6B}"/>
-    <hyperlink ref="C9" r:id="rId2" xr:uid="{E53C4E7C-62C1-480C-9CE1-D8F02AF8293F}"/>
-    <hyperlink ref="B10" r:id="rId3" xr:uid="{534D4B34-92AF-4AA1-B22A-0144DF92975F}"/>
-    <hyperlink ref="D9" r:id="rId4" xr:uid="{8DF7DE2D-DB4B-4DCF-901E-9015B764C84A}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId5"/>
-  <legacyDrawing r:id="rId6"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -1180,6 +1157,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010070B502A968965242AD1F25ACB97C8B93" ma:contentTypeVersion="6" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="20b2db34e954bf48f816685f8eee3e9a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="8f527fde-c8e9-4164-8da3-c17d2f59046f" xmlns:ns3="9238205a-6514-4f97-82f9-ec2a1068a494" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1f22045e64a90db03bf96faef922c3a8" ns2:_="" ns3:_="">
     <xsd:import namespace="8f527fde-c8e9-4164-8da3-c17d2f59046f"/>
@@ -1356,23 +1342,14 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CBC7A557-8DA3-4E06-822E-30426173EC2A}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{883DE857-F538-4ACA-9799-5011076E87C3}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{347CD3A9-9FDE-4F4F-B920-A80BEC3A8DD8}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{347CD3A9-9FDE-4F4F-B920-A80BEC3A8DD8}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{883DE857-F538-4ACA-9799-5011076E87C3}"/>
 </file>
</xml_diff>